<commit_message>
update of notes 4/23
</commit_message>
<xml_diff>
--- a/SexBehavior.xlsx
+++ b/SexBehavior.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\16093\Desktop\Webster Research\florisuga_sex_behavior\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E685D0D-5E19-438C-969F-F9F77CE6B3F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B193A75B-07A0-4AE4-AC53-6F2580F4FEEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{2B2F20DF-D7E1-944E-8139-D68C9E5E0917}"/>
+    <workbookView xWindow="-5693" yWindow="1567" windowWidth="12200" windowHeight="10073" xr2:uid="{2B2F20DF-D7E1-944E-8139-D68C9E5E0917}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="52">
   <si>
     <t>trial_num</t>
   </si>
@@ -173,7 +173,22 @@
     <t>10:49 (diff bird)</t>
   </si>
   <si>
-    <t>practice sentence</t>
+    <t>10:06 R, NA L</t>
+  </si>
+  <si>
+    <t>NA either</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NA </t>
+  </si>
+  <si>
+    <t>R (assuming)</t>
+  </si>
+  <si>
+    <t>L (assuming)</t>
+  </si>
+  <si>
+    <t>copul (maybe)</t>
   </si>
 </sst>
 </file>
@@ -209,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -225,6 +240,9 @@
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -540,10 +558,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C4875E9-3DAD-4141-A1E6-18F661E94E2F}">
-  <dimension ref="A1:I90"/>
+  <dimension ref="A1:I108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="C89" sqref="C89"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="A89" sqref="A89:A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
@@ -3105,13 +3123,455 @@
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A89" t="s">
+      <c r="A89" s="8">
+        <v>87</v>
+      </c>
+      <c r="B89" s="7">
+        <v>0.39999999999999997</v>
+      </c>
+      <c r="C89" s="4">
+        <v>1</v>
+      </c>
+      <c r="D89" s="4">
+        <v>1</v>
+      </c>
+      <c r="E89" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G89" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H89" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A90" s="8">
+        <v>91</v>
+      </c>
+      <c r="B90" s="7">
+        <v>0.44513888888888892</v>
+      </c>
+      <c r="C90" s="4">
+        <v>1</v>
+      </c>
+      <c r="D90" s="4">
+        <v>1</v>
+      </c>
+      <c r="E90" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F90" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G90" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="G89" s="4"/>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="G90" s="4"/>
+      <c r="H90" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A91" s="8">
+        <v>91</v>
+      </c>
+      <c r="B91" s="7">
+        <v>0.44513888888888892</v>
+      </c>
+      <c r="C91" s="4">
+        <v>1</v>
+      </c>
+      <c r="D91" s="4">
+        <v>2</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G91" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="H91" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A92" s="8">
+        <v>93</v>
+      </c>
+      <c r="B92" s="7">
+        <v>0.35694444444444445</v>
+      </c>
+      <c r="C92" s="4">
+        <v>1</v>
+      </c>
+      <c r="D92" s="4">
+        <v>1</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G92" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H92" s="7">
+        <v>0.3659722222222222</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A93" s="8">
+        <v>93</v>
+      </c>
+      <c r="B93" s="7">
+        <v>0.35694444444444445</v>
+      </c>
+      <c r="C93" s="4">
+        <v>1</v>
+      </c>
+      <c r="D93" s="4">
+        <v>2</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F93" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G93" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H93" s="7">
+        <v>0.3659722222222222</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A94" s="8">
+        <v>93</v>
+      </c>
+      <c r="B94" s="7">
+        <v>0.35694444444444445</v>
+      </c>
+      <c r="C94" s="4">
+        <v>1</v>
+      </c>
+      <c r="D94" s="4">
+        <v>3</v>
+      </c>
+      <c r="E94" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F94" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G94" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H94" s="7">
+        <v>0.3611111111111111</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A95" s="8">
+        <v>93</v>
+      </c>
+      <c r="B95" s="7">
+        <v>0.3659722222222222</v>
+      </c>
+      <c r="C95" s="4">
+        <v>2</v>
+      </c>
+      <c r="D95" s="4">
+        <v>1</v>
+      </c>
+      <c r="E95" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F95" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G95" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H95" s="7">
+        <v>0.38055555555555554</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A96" s="8">
+        <v>93</v>
+      </c>
+      <c r="B96" s="7">
+        <v>0.37013888888888885</v>
+      </c>
+      <c r="C96" s="4">
+        <v>3</v>
+      </c>
+      <c r="D96" s="4">
+        <v>1</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F96" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G96" s="7">
+        <v>0.3659722222222222</v>
+      </c>
+      <c r="H96" s="7">
+        <v>0.38055555555555554</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A97" s="8">
+        <v>94</v>
+      </c>
+      <c r="B97" s="7">
+        <v>0.35347222222222219</v>
+      </c>
+      <c r="C97" s="4">
+        <v>1</v>
+      </c>
+      <c r="D97" s="4">
+        <v>1</v>
+      </c>
+      <c r="E97" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F97" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G97" s="7">
+        <v>0.34236111111111112</v>
+      </c>
+      <c r="H97" s="7">
+        <v>0.35902777777777778</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A98" s="8">
+        <v>94</v>
+      </c>
+      <c r="B98" s="7">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="C98" s="4">
+        <v>2</v>
+      </c>
+      <c r="D98" s="4">
+        <v>1</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F98" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G98" s="7">
+        <v>0.37986111111111115</v>
+      </c>
+      <c r="H98" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A99" s="8">
+        <v>94</v>
+      </c>
+      <c r="B99" s="7">
+        <v>0.39513888888888887</v>
+      </c>
+      <c r="C99" s="4">
+        <v>3</v>
+      </c>
+      <c r="D99" s="4">
+        <v>1</v>
+      </c>
+      <c r="E99" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F99" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G99" s="7">
+        <v>0.37986111111111115</v>
+      </c>
+      <c r="H99" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A100" s="8">
+        <v>94</v>
+      </c>
+      <c r="B100" s="7">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="C100" s="4">
+        <v>4</v>
+      </c>
+      <c r="D100" s="4">
+        <v>1</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F100" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G100" s="7">
+        <v>0.37986111111111115</v>
+      </c>
+      <c r="H100" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A101" s="8">
+        <v>94</v>
+      </c>
+      <c r="B101" s="7">
+        <v>0.3979166666666667</v>
+      </c>
+      <c r="C101" s="4">
+        <v>5</v>
+      </c>
+      <c r="D101" s="4">
+        <v>1</v>
+      </c>
+      <c r="E101" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F101" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G101" s="7">
+        <v>0.37986111111111115</v>
+      </c>
+      <c r="H101" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A102" s="8">
+        <v>94</v>
+      </c>
+      <c r="B102" s="7">
+        <v>0.43263888888888885</v>
+      </c>
+      <c r="C102" s="4">
+        <v>6</v>
+      </c>
+      <c r="D102" s="4">
+        <v>1</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F102" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G102" s="7">
+        <v>0.39930555555555558</v>
+      </c>
+      <c r="H102" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A103" s="8">
+        <v>98</v>
+      </c>
+      <c r="B103" s="7">
+        <v>0.37916666666666665</v>
+      </c>
+      <c r="C103" s="4">
+        <v>1</v>
+      </c>
+      <c r="D103" s="4">
+        <v>1</v>
+      </c>
+      <c r="E103" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F103" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G103" s="7">
+        <v>0.37847222222222227</v>
+      </c>
+      <c r="H103" s="7">
+        <v>0.40486111111111112</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A104" s="8">
+        <v>98</v>
+      </c>
+      <c r="B104" s="7">
+        <v>0.38055555555555554</v>
+      </c>
+      <c r="C104" s="4">
+        <v>2</v>
+      </c>
+      <c r="D104" s="4">
+        <v>1</v>
+      </c>
+      <c r="E104" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F104" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G104" s="7">
+        <v>0.37916666666666665</v>
+      </c>
+      <c r="H104" s="7">
+        <v>0.40486111111111112</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A105" s="8">
+        <v>98</v>
+      </c>
+      <c r="B105" s="7">
+        <v>0.40486111111111112</v>
+      </c>
+      <c r="C105" s="4">
+        <v>3</v>
+      </c>
+      <c r="D105" s="4">
+        <v>1</v>
+      </c>
+      <c r="E105" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F105" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G105" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H105" s="7">
+        <v>0.44236111111111115</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A106" s="8"/>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A107" s="8"/>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A108" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>